<commit_message>
Can now read from excel and connect to email server. Will try to get the template to work now.
</commit_message>
<xml_diff>
--- a/Files/receivers.xlsx
+++ b/Files/receivers.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0811CD81-35B3-47D9-A257-A4A65874C71C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{65D8869B-E0A8-4194-A9AB-6AD4B5DF0951}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -23,22 +23,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>swag</t>
-  </si>
-  <si>
-    <t>humble</t>
-  </si>
-  <si>
-    <t>boii</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>Username:</t>
   </si>
   <si>
     <t>Password:</t>
+  </si>
+  <si>
+    <t>snirrfakturor</t>
+  </si>
+  <si>
+    <t>IrrSnirr96</t>
+  </si>
+  <si>
+    <t>Receiver Email</t>
+  </si>
+  <si>
+    <t>Subject</t>
   </si>
 </sst>
 </file>
@@ -371,26 +371,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -402,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C61B70-10F6-4405-8F75-2DD4AC55BAC6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -413,15 +410,19 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">

</xml_diff>

<commit_message>
Everything seems to work, need to write some comments and readme
</commit_message>
<xml_diff>
--- a/Files/receivers.xlsx
+++ b/Files/receivers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{65D8869B-E0A8-4194-A9AB-6AD4B5DF0951}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0958A2DD-7F45-41BE-9754-74772D65E172}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,18 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username:</t>
   </si>
   <si>
     <t>Password:</t>
-  </si>
-  <si>
-    <t>snirrfakturor</t>
-  </si>
-  <si>
-    <t>IrrSnirr96</t>
   </si>
   <si>
     <t>Receiver Email</t>
@@ -45,10 +39,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,14 +79,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -371,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -384,11 +389,20 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -400,33 +414,29 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>